<commit_message>
Allow dink dialogue in options.
</commit_message>
<xml_diff>
--- a/examples/test-js/dink-content/main-loc.xlsx
+++ b/examples/test-js/dink-content/main-loc.xlsx
@@ -28,18 +28,219 @@
     <x:t>Comments</x:t>
   </x:si>
   <x:si>
+    <x:t>main_Main_S72S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pick a thing to do...</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_QU2R</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trigger a Bark for Fred</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_X20S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trigger some not-Dink</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_OQ5O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Talk to Laura</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_NEAB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Some Comment Tests</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_AD94</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test Scene1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Main_768S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>You go to a completely separate file, scene1.ink!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_NotDink_4ZS7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>This is a test piece of Ink which doesn't have the Dink tag at the top.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_NotDink_D6LY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>So it works like normal Ink.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_CO2Z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hi, Laura here. What's up?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LAURA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_Hub_HUAV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>How are things, Laura?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_Hub_5T8A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oh, not too bad, thanks!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_Hub_RWJJ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>What's the weather like?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_Hub_J0MK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>It's pretty good today.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_Hub_CIMX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Raining as always.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_Hub_L3K7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dull, dull grey.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_LauraChat_Hub_MKGT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(Leave.)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_16U4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>We're testing some comments here.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Comment for a line. Another comment for the same line.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_G33S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>It'll only make sense if you export a recording script or the Dink structure.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_FF1T</x:t>
+  </x:si>
+  <x:si>
+    <x:t>This is another line.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>This comment goes to the voice actor. This comment goes to the localisers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_BQ1E</x:t>
+  </x:si>
+  <x:si>
+    <x:t>This is a loud line!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FRED</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fred is angry.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_IQIS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Glad that's over with!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_MP0B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Back</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_O037</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hey!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_UWZ2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stop poking me!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_1ZG8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Why do you keep doing that?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_JFG1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ignoring you. Gonna grab a beer.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_4444</x:t>
+  </x:si>
+  <x:si>
+    <x:t>What? I'm busy - Jim's here.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_X291</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I'm happy for you to poke him, really.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JIM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_L2SX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stop it!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_N07F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wow this is annoying!</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Part1_S494</x:t>
   </x:si>
   <x:si>
     <x:t>This is a block called Part1 in a scene.</x:t>
   </x:si>
   <x:si>
-    <x:t>FRED</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
     <x:t>scene1_Scene1_Part1_ICIG</x:t>
   </x:si>
   <x:si>
@@ -130,9 +331,6 @@
     <x:t>scene1_Scene1_Part4_PZV1</x:t>
   </x:si>
   <x:si>
-    <x:t>Back</x:t>
-  </x:si>
-  <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
   </x:si>
   <x:si>
@@ -161,204 +359,6 @@
   </x:si>
   <x:si>
     <x:t>scene1_OtherContent_VZWQ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Main_S72S</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pick a thing to do...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Main_QU2R</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trigger a Bark for Fred</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Main_X20S</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trigger some not-Dink</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Main_OQ5O</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Talk to Laura</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Main_NEAB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Some Comment Tests</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Main_AD94</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test Scene1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Main_768S</x:t>
-  </x:si>
-  <x:si>
-    <x:t>You go to a completely separate file, scene1.ink!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_NotDink_4ZS7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>This is a test piece of Ink which doesn't have the Dink tag at the top.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_NotDink_D6LY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>So it works like normal Ink.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_CO2Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hi, Laura here. What's up?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LAURA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_Hub_HUAV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>How are things, Laura?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_Hub_5T8A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Oh, not too bad, thanks!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_Hub_RWJJ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>What's the weather like?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_Hub_J0MK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>It's pretty good today.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_Hub_CIMX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Raining as always.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_Hub_L3K7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dull, dull grey.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_LauraChat_Hub_MKGT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(Leave.)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_TestScene_16U4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>We're testing some comments here.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Comment for a line. Another comment for the same line.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_TestScene_G33S</x:t>
-  </x:si>
-  <x:si>
-    <x:t>It'll only make sense if you export a recording script or the Dink structure.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_TestScene_FF1T</x:t>
-  </x:si>
-  <x:si>
-    <x:t>This is another line.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>This comment goes to the voice actor. This comment goes to the localisers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_TestScene_BQ1E</x:t>
-  </x:si>
-  <x:si>
-    <x:t>This is a loud line!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fred is angry.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_TestScene_IQIS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Glad that's over with!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_TestScene_MP0B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_O037</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hey!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_UWZ2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stop poking me!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_1ZG8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Why do you keep doing that?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_JFG1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ignoring you. Gonna grab a beer.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_4444</x:t>
-  </x:si>
-  <x:si>
-    <x:t>What? I'm busy - Jim's here.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_X291</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I'm happy for you to poke him, really.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>JIM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_L2SX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stop it!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_N07F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wow this is annoying!</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -789,273 +789,273 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="D2" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A3" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B3" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="C3" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A4" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B4" s="1" t="s">
-        <x:v>11</x:v>
-      </x:c>
       <x:c r="C4" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D4" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A5" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B5" s="1" t="s">
-        <x:v>13</x:v>
-      </x:c>
       <x:c r="C5" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D5" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A6" s="1" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="B6" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
       <x:c r="C6" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D6" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A7" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B7" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C7" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D7" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A8" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D8" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A9" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D9" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A10" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C10" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D10" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A11" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D11" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A12" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C12" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D12" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A13" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C13" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D13" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A14" s="1" t="s">
-        <x:v>33</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
-        <x:v>34</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C14" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D14" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A15" s="1" t="s">
-        <x:v>35</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>36</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D15" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A16" s="1" t="s">
-        <x:v>37</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
-        <x:v>38</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C16" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D16" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A17" s="1" t="s">
-        <x:v>39</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
-        <x:v>40</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C17" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D17" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A18" s="1" t="s">
-        <x:v>41</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C18" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D18" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A19" s="1" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B19" s="1" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C19" s="1" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D19" s="1" t="s">
         <x:v>42</x:v>
-      </x:c>
-      <x:c r="B19" s="1" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C19" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D19" s="1" t="s">
-        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A20" s="1" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B20" s="1" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="B20" s="1" t="s">
-        <x:v>45</x:v>
-      </x:c>
       <x:c r="C20" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D20" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A21" s="1" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B21" s="1" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="B21" s="1" t="s">
+      <x:c r="C21" s="1" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D21" s="1" t="s">
         <x:v>47</x:v>
-      </x:c>
-      <x:c r="C21" s="1" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D21" s="1" t="s">
-        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4" ht="13.5" customHeight="1">
@@ -1063,447 +1063,447 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="B22" s="1" t="s">
-        <x:v>45</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C22" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D22" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A23" s="1" t="s">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B23" s="1" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C23" s="1" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="C23" s="1" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="D23" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A24" s="1" t="s">
-        <x:v>51</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B24" s="1" t="s">
-        <x:v>52</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C24" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D24" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A25" s="1" t="s">
-        <x:v>53</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B25" s="1" t="s">
-        <x:v>54</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C25" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D25" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A26" s="1" t="s">
-        <x:v>55</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B26" s="1" t="s">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C26" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D26" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A27" s="1" t="s">
-        <x:v>57</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B27" s="1" t="s">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C27" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D27" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A28" s="1" t="s">
-        <x:v>59</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B28" s="1" t="s">
-        <x:v>60</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C28" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D28" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A29" s="1" t="s">
-        <x:v>61</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B29" s="1" t="s">
-        <x:v>62</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C29" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D29" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A30" s="1" t="s">
-        <x:v>63</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B30" s="1" t="s">
-        <x:v>64</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C30" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="D30" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A31" s="1" t="s">
-        <x:v>65</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B31" s="1" t="s">
-        <x:v>66</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C31" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D31" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A32" s="1" t="s">
-        <x:v>67</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B32" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C32" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D32" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A33" s="1" t="s">
-        <x:v>70</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B33" s="1" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C33" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D33" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A34" s="1" t="s">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B34" s="1" t="s">
-        <x:v>73</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C34" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D34" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A35" s="1" t="s">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B35" s="1" t="s">
-        <x:v>75</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C35" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D35" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A36" s="1" t="s">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B36" s="1" t="s">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C36" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D36" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A37" s="1" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B37" s="1" t="s">
-        <x:v>79</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C37" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D37" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A38" s="1" t="s">
-        <x:v>80</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="B38" s="1" t="s">
-        <x:v>81</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C38" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D38" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A39" s="1" t="s">
-        <x:v>82</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B39" s="1" t="s">
-        <x:v>83</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C39" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D39" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A40" s="1" t="s">
-        <x:v>84</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="B40" s="1" t="s">
-        <x:v>85</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C40" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D40" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A41" s="1" t="s">
-        <x:v>87</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="B41" s="1" t="s">
-        <x:v>88</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C41" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D41" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A42" s="1" t="s">
-        <x:v>89</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B42" s="1" t="s">
-        <x:v>90</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C42" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D42" s="1" t="s">
-        <x:v>91</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A43" s="1" t="s">
-        <x:v>92</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="B43" s="1" t="s">
-        <x:v>93</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C43" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D43" s="1" t="s">
-        <x:v>94</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A44" s="1" t="s">
-        <x:v>95</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="B44" s="1" t="s">
-        <x:v>96</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C44" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D44" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A45" s="1" t="s">
-        <x:v>97</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B45" s="1" t="s">
-        <x:v>38</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="C45" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D45" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A46" s="1" t="s">
-        <x:v>98</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="B46" s="1" t="s">
-        <x:v>99</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="C46" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D46" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A47" s="1" t="s">
-        <x:v>100</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="B47" s="1" t="s">
-        <x:v>101</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C47" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D47" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A48" s="1" t="s">
-        <x:v>102</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="B48" s="1" t="s">
-        <x:v>103</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C48" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D48" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A49" s="1" t="s">
-        <x:v>104</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="B49" s="1" t="s">
-        <x:v>105</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C49" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D49" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A50" s="1" t="s">
-        <x:v>106</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="B50" s="1" t="s">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="C50" s="1" t="s">
-        <x:v>6</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="D50" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A51" s="1" t="s">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="B51" s="1" t="s">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C51" s="1" t="s">
-        <x:v>110</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D51" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A52" s="1" t="s">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B52" s="1" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C52" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D52" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:4" ht="13.5" customHeight="1">
       <x:c r="A53" s="1" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="B53" s="1" t="s">
-        <x:v>114</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C53" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D53" s="1" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>